<commit_message>
correct Run Type entry in pacbio experiment run template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Experiment_run_Pacbio_v5_3_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Experiment_run_Pacbio_v5_3_0.xlsx
@@ -8,10 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Experiments" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Samples" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Index" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Experiments" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Samples" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Info" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Index" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="iSeq_flowcells" vbProcedure="false">#REF!</definedName>
@@ -32,7 +32,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>UFG</author>
+    <author>Unknown Author</author>
   </authors>
   <commentList>
     <comment ref="B6" authorId="0">
@@ -42,7 +42,6 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Illumina Flowcell Barcode</t>
         </r>
@@ -97,7 +96,7 @@
     <t xml:space="preserve">Run Type</t>
   </si>
   <si>
-    <t xml:space="preserve">Pacbio</t>
+    <t xml:space="preserve">PacBio</t>
   </si>
   <si>
     <t xml:space="preserve">*</t>
@@ -1505,7 +1504,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1843,8 +1841,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1856,7 +1960,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.52"/>
@@ -1968,7 +2072,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -4618,22 +4722,22 @@
     <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C7:C100" type="list">
       <formula1>Index!$F$2:$F$2</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D7:D100" type="list">
       <formula1>INDIRECT(SUBSTITUTE(INDEX(Index!$G$2:$G$2, MATCH(C7, Index!$F$2:$F$2, 0), 1), " ", "_"))</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H100" type="list">
       <formula1>Index!$D$2:$D$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4643,7 +4747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4655,7 +4759,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.84"/>
@@ -4716,7 +4820,7 @@
       </c>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
@@ -4760,7 +4864,6 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="0"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4772,7 +4875,6 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="0"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9114,38 +9216,38 @@
     <mergeCell ref="J3:K3"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K5:K100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K5:K100" type="list">
       <formula1>"12h,24h,30h"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5:D101" type="list">
       <formula1>Index!$B$2:$B$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A5:A100" type="list">
       <formula1>Experiments!$A$7:$A$106</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5:I100" type="list">
       <formula1>Index!$E$2:$E$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E101" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E5:E101" type="none">
       <formula1>Index!$B$2:$B$97</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G101:G1000" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G101:G1000" type="list">
       <formula1>"1,2,3,4,5,6,7,8,A01,A02,A03,A04,A05,A06,A07,A08"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G5:G100" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G5:G100" type="list">
       <formula1>Index!$A$2:$A$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -9154,7 +9256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9164,7 +9266,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.68"/>
   </cols>
@@ -9387,7 +9489,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -9396,7 +9498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -9406,7 +9508,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.51953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.83"/>
@@ -9416,8 +9518,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="1019" style="1" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1019" style="1" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12311,7 +12412,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>